<commit_message>
add map enemy factory
</commit_message>
<xml_diff>
--- a/Assets/DataTable/Quest_List.xlsx
+++ b/Assets/DataTable/Quest_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kk/Desktop/Project/2/Funkeln/Assets/DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5BF761-BA7A-404F-BBBD-037CE627B961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9B5360-A1B8-554F-8C43-6CE6C46FE012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{9399BE26-D56F-4B5E-9B99-03A6601666B1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>MapName</t>
   </si>
@@ -72,13 +72,19 @@
     <t>MapID</t>
   </si>
   <si>
-    <t>EnrmyPlace</t>
-  </si>
-  <si>
     <t>BossFlag</t>
   </si>
   <si>
     <t>EnemyID1</t>
+  </si>
+  <si>
+    <t>EnemyStage1</t>
+  </si>
+  <si>
+    <t>EnemyStage2</t>
+  </si>
+  <si>
+    <t>EnemyStage3</t>
   </si>
 </sst>
 </file>
@@ -535,17 +541,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F51082F-399C-438E-9AF8-894D55DD6386}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="22.1640625" bestFit="1" customWidth="1"/>
@@ -553,7 +559,7 @@
     <col min="11" max="11" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29" thickBot="1">
+    <row r="1" spans="1:12" ht="29" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -564,28 +570,34 @@
         <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12">
       <c r="A2" s="6">
         <v>101</v>
       </c>
@@ -596,28 +608,34 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
+        <v>2</v>
+      </c>
+      <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>104000</v>
-      </c>
-      <c r="G2">
-        <v>104000</v>
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>104000</v>
+        <v>4000</v>
       </c>
       <c r="I2">
-        <v>104000</v>
+        <v>5000</v>
       </c>
       <c r="J2">
+        <v>4000</v>
+      </c>
+      <c r="K2">
+        <v>5000</v>
+      </c>
+      <c r="L2">
         <v>104000</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="A3" s="6">
         <v>102</v>
       </c>
@@ -628,16 +646,16 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
+        <v>2</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>104000</v>
-      </c>
-      <c r="G3">
-        <v>104000</v>
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
       </c>
       <c r="H3">
         <v>104000</v>
@@ -648,8 +666,14 @@
       <c r="J3">
         <v>104000</v>
       </c>
+      <c r="K3">
+        <v>104000</v>
+      </c>
+      <c r="L3">
+        <v>104000</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="A4" s="6">
         <v>103</v>
       </c>
@@ -660,16 +684,16 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
+        <v>2</v>
+      </c>
+      <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>104000</v>
-      </c>
-      <c r="G4">
-        <v>104000</v>
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
       </c>
       <c r="H4">
         <v>104000</v>
@@ -680,8 +704,14 @@
       <c r="J4">
         <v>104000</v>
       </c>
+      <c r="K4">
+        <v>104000</v>
+      </c>
+      <c r="L4">
+        <v>104000</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:12">
       <c r="F5" s="4"/>
     </row>
   </sheetData>

</xml_diff>